<commit_message>
permission to dance, hard 노트 수정
</commit_message>
<xml_diff>
--- a/NoteMaps/PTD_BTS.xlsx
+++ b/NoteMaps/PTD_BTS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eogus\source\repos\RhythmGame\NoteMaps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{311E3B77-A88B-4DA4-8B84-FB7F2EBC6850}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29A93F82-9052-4D23-9FAD-B184B2EAC20E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{FBD1AADC-AD03-4139-A607-30D499883534}"/>
   </bookViews>
@@ -482,8 +482,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{597C38B7-F2CF-4951-BED7-7D28309F5979}">
   <dimension ref="A1:G1063"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1034" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G1051" sqref="G1051"/>
+    <sheetView tabSelected="1" topLeftCell="A841" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H806" sqref="H806"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -8658,8 +8658,8 @@
       <c r="C360" s="2">
         <v>1</v>
       </c>
-      <c r="D360" s="1">
-        <v>1</v>
+      <c r="D360">
+        <v>0</v>
       </c>
       <c r="E360">
         <v>0</v>
@@ -11418,8 +11418,8 @@
       <c r="C480" s="2">
         <v>1</v>
       </c>
-      <c r="D480" s="1">
-        <v>1</v>
+      <c r="D480">
+        <v>0</v>
       </c>
       <c r="E480">
         <v>0</v>
@@ -11789,8 +11789,8 @@
       <c r="D496">
         <v>0</v>
       </c>
-      <c r="E496">
-        <v>0</v>
+      <c r="E496" s="1">
+        <v>1</v>
       </c>
       <c r="F496">
         <v>0</v>
@@ -12157,8 +12157,8 @@
       <c r="D512">
         <v>0</v>
       </c>
-      <c r="E512">
-        <v>0</v>
+      <c r="E512" s="1">
+        <v>1</v>
       </c>
       <c r="F512" s="1">
         <v>1</v>
@@ -13074,17 +13074,17 @@
       <c r="C552" s="2">
         <v>1</v>
       </c>
-      <c r="D552">
-        <v>0</v>
-      </c>
-      <c r="E552" s="1">
-        <v>1</v>
+      <c r="D552" s="1">
+        <v>1</v>
+      </c>
+      <c r="E552">
+        <v>0</v>
       </c>
       <c r="F552" s="1">
         <v>1</v>
       </c>
-      <c r="G552" s="1">
-        <v>1</v>
+      <c r="G552">
+        <v>0</v>
       </c>
     </row>
     <row r="553" spans="1:7" x14ac:dyDescent="0.4">
@@ -13261,14 +13261,14 @@
       <c r="D560">
         <v>0</v>
       </c>
-      <c r="E560">
-        <v>0</v>
+      <c r="E560" s="1">
+        <v>1</v>
       </c>
       <c r="F560">
         <v>0</v>
       </c>
-      <c r="G560" s="1">
-        <v>1</v>
+      <c r="G560">
+        <v>0</v>
       </c>
     </row>
     <row r="561" spans="1:7" x14ac:dyDescent="0.4">
@@ -13353,14 +13353,14 @@
       <c r="D564">
         <v>0</v>
       </c>
-      <c r="E564" s="1">
-        <v>1</v>
-      </c>
-      <c r="F564">
-        <v>0</v>
-      </c>
-      <c r="G564" s="1">
-        <v>1</v>
+      <c r="E564">
+        <v>0</v>
+      </c>
+      <c r="F564" s="1">
+        <v>1</v>
+      </c>
+      <c r="G564">
+        <v>0</v>
       </c>
     </row>
     <row r="565" spans="1:7" x14ac:dyDescent="0.4">
@@ -13448,11 +13448,11 @@
       <c r="E568">
         <v>0</v>
       </c>
-      <c r="F568">
-        <v>0</v>
-      </c>
-      <c r="G568" s="1">
-        <v>1</v>
+      <c r="F568" s="1">
+        <v>1</v>
+      </c>
+      <c r="G568">
+        <v>0</v>
       </c>
     </row>
     <row r="569" spans="1:7" x14ac:dyDescent="0.4">
@@ -13534,11 +13534,11 @@
       <c r="C572" s="2">
         <v>5</v>
       </c>
-      <c r="D572">
-        <v>0</v>
-      </c>
-      <c r="E572" s="1">
-        <v>1</v>
+      <c r="D572" s="1">
+        <v>1</v>
+      </c>
+      <c r="E572">
+        <v>0</v>
       </c>
       <c r="F572">
         <v>0</v>
@@ -13586,8 +13586,8 @@
       <c r="E574">
         <v>0</v>
       </c>
-      <c r="F574" s="1">
-        <v>1</v>
+      <c r="F574">
+        <v>0</v>
       </c>
       <c r="G574">
         <v>0</v>
@@ -13629,14 +13629,14 @@
       <c r="D576">
         <v>0</v>
       </c>
-      <c r="E576">
-        <v>0</v>
+      <c r="E576" s="1">
+        <v>1</v>
       </c>
       <c r="F576">
         <v>0</v>
       </c>
-      <c r="G576" s="1">
-        <v>1</v>
+      <c r="G576">
+        <v>0</v>
       </c>
     </row>
     <row r="577" spans="1:7" x14ac:dyDescent="0.4">
@@ -13718,17 +13718,17 @@
       <c r="C580" s="2">
         <v>5</v>
       </c>
-      <c r="D580" s="1">
-        <v>1</v>
+      <c r="D580">
+        <v>0</v>
       </c>
       <c r="E580">
         <v>0</v>
       </c>
-      <c r="F580">
-        <v>0</v>
-      </c>
-      <c r="G580" s="1">
-        <v>1</v>
+      <c r="F580" s="1">
+        <v>1</v>
+      </c>
+      <c r="G580">
+        <v>0</v>
       </c>
     </row>
     <row r="581" spans="1:7" x14ac:dyDescent="0.4">
@@ -13816,8 +13816,8 @@
       <c r="E584">
         <v>0</v>
       </c>
-      <c r="F584">
-        <v>0</v>
+      <c r="F584" s="1">
+        <v>1</v>
       </c>
       <c r="G584">
         <v>0</v>
@@ -13859,8 +13859,8 @@
       <c r="D586">
         <v>0</v>
       </c>
-      <c r="E586" s="1">
-        <v>1</v>
+      <c r="E586">
+        <v>0</v>
       </c>
       <c r="F586">
         <v>0</v>
@@ -13997,14 +13997,14 @@
       <c r="D592">
         <v>0</v>
       </c>
-      <c r="E592">
-        <v>0</v>
+      <c r="E592" s="1">
+        <v>1</v>
       </c>
       <c r="F592">
         <v>0</v>
       </c>
-      <c r="G592" s="1">
-        <v>1</v>
+      <c r="G592">
+        <v>0</v>
       </c>
     </row>
     <row r="593" spans="1:7" x14ac:dyDescent="0.4">
@@ -14086,8 +14086,8 @@
       <c r="C596" s="2">
         <v>5</v>
       </c>
-      <c r="D596" s="1">
-        <v>1</v>
+      <c r="D596">
+        <v>0</v>
       </c>
       <c r="E596">
         <v>0</v>
@@ -14178,8 +14178,8 @@
       <c r="C600" s="2">
         <v>1</v>
       </c>
-      <c r="D600" s="1">
-        <v>1</v>
+      <c r="D600">
+        <v>0</v>
       </c>
       <c r="E600">
         <v>0</v>
@@ -14227,8 +14227,8 @@
       <c r="D602">
         <v>0</v>
       </c>
-      <c r="E602" s="1">
-        <v>1</v>
+      <c r="E602">
+        <v>0</v>
       </c>
       <c r="F602">
         <v>0</v>
@@ -14270,8 +14270,8 @@
       <c r="C604" s="2">
         <v>5</v>
       </c>
-      <c r="D604">
-        <v>0</v>
+      <c r="D604" s="1">
+        <v>1</v>
       </c>
       <c r="E604">
         <v>0</v>
@@ -14365,14 +14365,14 @@
       <c r="D608">
         <v>0</v>
       </c>
-      <c r="E608">
-        <v>0</v>
+      <c r="E608" s="1">
+        <v>1</v>
       </c>
       <c r="F608">
         <v>0</v>
       </c>
-      <c r="G608">
-        <v>0</v>
+      <c r="G608" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="609" spans="1:7" x14ac:dyDescent="0.4">
@@ -14457,11 +14457,11 @@
       <c r="D612" s="1">
         <v>1</v>
       </c>
-      <c r="E612" s="1">
-        <v>1</v>
-      </c>
-      <c r="F612">
-        <v>0</v>
+      <c r="E612">
+        <v>0</v>
+      </c>
+      <c r="F612" s="1">
+        <v>1</v>
       </c>
       <c r="G612">
         <v>0</v>
@@ -14601,8 +14601,8 @@
       <c r="F618">
         <v>0</v>
       </c>
-      <c r="G618" s="1">
-        <v>1</v>
+      <c r="G618">
+        <v>0</v>
       </c>
     </row>
     <row r="619" spans="1:7" x14ac:dyDescent="0.4">
@@ -14647,8 +14647,8 @@
       <c r="F620">
         <v>0</v>
       </c>
-      <c r="G620">
-        <v>0</v>
+      <c r="G620" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="621" spans="1:7" x14ac:dyDescent="0.4">
@@ -14914,8 +14914,8 @@
       <c r="C632" s="2">
         <v>1</v>
       </c>
-      <c r="D632" s="1">
-        <v>1</v>
+      <c r="D632">
+        <v>0</v>
       </c>
       <c r="E632">
         <v>0</v>
@@ -14966,8 +14966,8 @@
       <c r="E634">
         <v>0</v>
       </c>
-      <c r="F634" s="1">
-        <v>1</v>
+      <c r="F634">
+        <v>0</v>
       </c>
       <c r="G634">
         <v>0</v>
@@ -15012,8 +15012,8 @@
       <c r="E636">
         <v>0</v>
       </c>
-      <c r="F636">
-        <v>0</v>
+      <c r="F636" s="1">
+        <v>1</v>
       </c>
       <c r="G636">
         <v>0</v>
@@ -15104,8 +15104,8 @@
       <c r="E640" s="1">
         <v>1</v>
       </c>
-      <c r="F640" s="1">
-        <v>1</v>
+      <c r="F640">
+        <v>0</v>
       </c>
       <c r="G640">
         <v>0</v>
@@ -15196,8 +15196,8 @@
       <c r="E644">
         <v>0</v>
       </c>
-      <c r="F644">
-        <v>0</v>
+      <c r="F644" s="1">
+        <v>1</v>
       </c>
       <c r="G644">
         <v>0</v>
@@ -15282,14 +15282,14 @@
       <c r="C648" s="2">
         <v>1</v>
       </c>
-      <c r="D648">
-        <v>0</v>
+      <c r="D648" s="1">
+        <v>1</v>
       </c>
       <c r="E648">
         <v>0</v>
       </c>
-      <c r="F648" s="1">
-        <v>1</v>
+      <c r="F648">
+        <v>0</v>
       </c>
       <c r="G648">
         <v>0</v>
@@ -15337,8 +15337,8 @@
       <c r="F650">
         <v>0</v>
       </c>
-      <c r="G650" s="1">
-        <v>1</v>
+      <c r="G650">
+        <v>0</v>
       </c>
     </row>
     <row r="651" spans="1:7" x14ac:dyDescent="0.4">
@@ -15650,8 +15650,8 @@
       <c r="C664" s="2">
         <v>1</v>
       </c>
-      <c r="D664">
-        <v>0</v>
+      <c r="D664" s="1">
+        <v>1</v>
       </c>
       <c r="E664">
         <v>0</v>
@@ -16024,11 +16024,11 @@
       <c r="E680">
         <v>0</v>
       </c>
-      <c r="F680">
-        <v>0</v>
-      </c>
-      <c r="G680" s="1">
-        <v>1</v>
+      <c r="F680" s="1">
+        <v>1</v>
+      </c>
+      <c r="G680">
+        <v>0</v>
       </c>
     </row>
     <row r="681" spans="1:7" x14ac:dyDescent="0.4">
@@ -16067,8 +16067,8 @@
       <c r="D682">
         <v>0</v>
       </c>
-      <c r="E682" s="1">
-        <v>1</v>
+      <c r="E682">
+        <v>0</v>
       </c>
       <c r="F682">
         <v>0</v>
@@ -16113,14 +16113,14 @@
       <c r="D684">
         <v>0</v>
       </c>
-      <c r="E684">
-        <v>0</v>
+      <c r="E684" s="1">
+        <v>1</v>
       </c>
       <c r="F684">
         <v>0</v>
       </c>
-      <c r="G684" s="1">
-        <v>1</v>
+      <c r="G684">
+        <v>0</v>
       </c>
     </row>
     <row r="685" spans="1:7" x14ac:dyDescent="0.4">
@@ -16303,8 +16303,8 @@
       <c r="F692">
         <v>0</v>
       </c>
-      <c r="G692" s="1">
-        <v>1</v>
+      <c r="G692">
+        <v>0</v>
       </c>
     </row>
     <row r="693" spans="1:7" x14ac:dyDescent="0.4">
@@ -16392,11 +16392,11 @@
       <c r="E696">
         <v>0</v>
       </c>
-      <c r="F696">
-        <v>0</v>
-      </c>
-      <c r="G696" s="1">
-        <v>1</v>
+      <c r="F696" s="1">
+        <v>1</v>
+      </c>
+      <c r="G696">
+        <v>0</v>
       </c>
     </row>
     <row r="697" spans="1:7" x14ac:dyDescent="0.4">
@@ -16481,11 +16481,11 @@
       <c r="D700">
         <v>0</v>
       </c>
-      <c r="E700" s="1">
-        <v>1</v>
-      </c>
-      <c r="F700">
-        <v>0</v>
+      <c r="E700">
+        <v>0</v>
+      </c>
+      <c r="F700" s="1">
+        <v>1</v>
       </c>
       <c r="G700">
         <v>0</v>
@@ -16530,8 +16530,8 @@
       <c r="E702">
         <v>0</v>
       </c>
-      <c r="F702" s="1">
-        <v>1</v>
+      <c r="F702">
+        <v>0</v>
       </c>
       <c r="G702">
         <v>0</v>
@@ -16573,14 +16573,14 @@
       <c r="D704">
         <v>0</v>
       </c>
-      <c r="E704" s="1">
-        <v>1</v>
+      <c r="E704">
+        <v>0</v>
       </c>
       <c r="F704">
         <v>0</v>
       </c>
-      <c r="G704">
-        <v>0</v>
+      <c r="G704" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="705" spans="1:7" x14ac:dyDescent="0.4">
@@ -16760,8 +16760,8 @@
       <c r="E712">
         <v>0</v>
       </c>
-      <c r="F712">
-        <v>0</v>
+      <c r="F712" s="1">
+        <v>1</v>
       </c>
       <c r="G712">
         <v>0</v>
@@ -16803,8 +16803,8 @@
       <c r="D714">
         <v>0</v>
       </c>
-      <c r="E714" s="1">
-        <v>1</v>
+      <c r="E714">
+        <v>0</v>
       </c>
       <c r="F714">
         <v>0</v>
@@ -16849,14 +16849,14 @@
       <c r="D716">
         <v>0</v>
       </c>
-      <c r="E716">
-        <v>0</v>
+      <c r="E716" s="1">
+        <v>1</v>
       </c>
       <c r="F716">
         <v>0</v>
       </c>
-      <c r="G716" s="1">
-        <v>1</v>
+      <c r="G716">
+        <v>0</v>
       </c>
     </row>
     <row r="717" spans="1:7" x14ac:dyDescent="0.4">
@@ -16944,11 +16944,11 @@
       <c r="E720">
         <v>0</v>
       </c>
-      <c r="F720" s="1">
-        <v>1</v>
-      </c>
-      <c r="G720">
-        <v>0</v>
+      <c r="F720">
+        <v>0</v>
+      </c>
+      <c r="G720" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="721" spans="1:7" x14ac:dyDescent="0.4">
@@ -17036,8 +17036,8 @@
       <c r="E724">
         <v>0</v>
       </c>
-      <c r="F724" s="1">
-        <v>1</v>
+      <c r="F724">
+        <v>0</v>
       </c>
       <c r="G724">
         <v>0</v>
@@ -17269,8 +17269,8 @@
       <c r="F734">
         <v>0</v>
       </c>
-      <c r="G734" s="1">
-        <v>1</v>
+      <c r="G734">
+        <v>0</v>
       </c>
     </row>
     <row r="735" spans="1:7" x14ac:dyDescent="0.4">
@@ -17312,11 +17312,11 @@
       <c r="E736" s="1">
         <v>1</v>
       </c>
-      <c r="F736" s="1">
-        <v>1</v>
-      </c>
-      <c r="G736">
-        <v>0</v>
+      <c r="F736">
+        <v>0</v>
+      </c>
+      <c r="G736" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="737" spans="1:7" x14ac:dyDescent="0.4">
@@ -17404,8 +17404,8 @@
       <c r="E740">
         <v>0</v>
       </c>
-      <c r="F740">
-        <v>0</v>
+      <c r="F740" s="1">
+        <v>1</v>
       </c>
       <c r="G740">
         <v>0</v>
@@ -17545,8 +17545,8 @@
       <c r="F746">
         <v>0</v>
       </c>
-      <c r="G746" s="1">
-        <v>1</v>
+      <c r="G746">
+        <v>0</v>
       </c>
     </row>
     <row r="747" spans="1:7" x14ac:dyDescent="0.4">
@@ -17585,8 +17585,8 @@
       <c r="D748">
         <v>0</v>
       </c>
-      <c r="E748">
-        <v>0</v>
+      <c r="E748" s="1">
+        <v>1</v>
       </c>
       <c r="F748">
         <v>0</v>
@@ -17677,14 +17677,14 @@
       <c r="D752">
         <v>0</v>
       </c>
-      <c r="E752" s="1">
-        <v>1</v>
+      <c r="E752">
+        <v>0</v>
       </c>
       <c r="F752">
         <v>0</v>
       </c>
-      <c r="G752">
-        <v>0</v>
+      <c r="G752" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="753" spans="1:7" x14ac:dyDescent="0.4">
@@ -17766,14 +17766,14 @@
       <c r="C756" s="2">
         <v>5</v>
       </c>
-      <c r="D756">
-        <v>0</v>
+      <c r="D756" s="1">
+        <v>1</v>
       </c>
       <c r="E756">
         <v>0</v>
       </c>
-      <c r="F756" s="1">
-        <v>1</v>
+      <c r="F756">
+        <v>0</v>
       </c>
       <c r="G756">
         <v>0</v>
@@ -17864,8 +17864,8 @@
       <c r="E760">
         <v>0</v>
       </c>
-      <c r="F760" s="1">
-        <v>1</v>
+      <c r="F760">
+        <v>0</v>
       </c>
       <c r="G760">
         <v>0</v>
@@ -17910,8 +17910,8 @@
       <c r="E762">
         <v>0</v>
       </c>
-      <c r="F762" s="1">
-        <v>1</v>
+      <c r="F762">
+        <v>0</v>
       </c>
       <c r="G762">
         <v>0</v>
@@ -17956,8 +17956,8 @@
       <c r="E764">
         <v>0</v>
       </c>
-      <c r="F764">
-        <v>0</v>
+      <c r="F764" s="1">
+        <v>1</v>
       </c>
       <c r="G764">
         <v>0</v>
@@ -18045,14 +18045,14 @@
       <c r="D768">
         <v>0</v>
       </c>
-      <c r="E768" s="1">
-        <v>1</v>
-      </c>
-      <c r="F768" s="1">
-        <v>1</v>
-      </c>
-      <c r="G768">
-        <v>0</v>
+      <c r="E768">
+        <v>0</v>
+      </c>
+      <c r="F768">
+        <v>0</v>
+      </c>
+      <c r="G768" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="769" spans="1:7" x14ac:dyDescent="0.4">
@@ -18134,14 +18134,14 @@
       <c r="C772" s="2">
         <v>5</v>
       </c>
-      <c r="D772">
-        <v>0</v>
+      <c r="D772" s="1">
+        <v>1</v>
       </c>
       <c r="E772">
         <v>0</v>
       </c>
-      <c r="F772">
-        <v>0</v>
+      <c r="F772" s="1">
+        <v>1</v>
       </c>
       <c r="G772">
         <v>0</v>
@@ -18232,8 +18232,8 @@
       <c r="E776">
         <v>0</v>
       </c>
-      <c r="F776">
-        <v>0</v>
+      <c r="F776" s="1">
+        <v>1</v>
       </c>
       <c r="G776">
         <v>0</v>
@@ -18324,8 +18324,8 @@
       <c r="E780">
         <v>0</v>
       </c>
-      <c r="F780" s="1">
-        <v>1</v>
+      <c r="F780">
+        <v>0</v>
       </c>
       <c r="G780">
         <v>0</v>
@@ -18465,8 +18465,8 @@
       <c r="F786">
         <v>0</v>
       </c>
-      <c r="G786" s="1">
-        <v>1</v>
+      <c r="G786">
+        <v>0</v>
       </c>
     </row>
     <row r="787" spans="1:7" x14ac:dyDescent="0.4">
@@ -18502,11 +18502,11 @@
       <c r="C788" s="2">
         <v>5</v>
       </c>
-      <c r="D788" s="1">
-        <v>1</v>
-      </c>
-      <c r="E788">
-        <v>0</v>
+      <c r="D788">
+        <v>0</v>
+      </c>
+      <c r="E788" s="1">
+        <v>1</v>
       </c>
       <c r="F788" s="1">
         <v>1</v>
@@ -18781,14 +18781,14 @@
       <c r="D800">
         <v>0</v>
       </c>
-      <c r="E800" s="1">
-        <v>1</v>
+      <c r="E800">
+        <v>0</v>
       </c>
       <c r="F800" s="1">
         <v>1</v>
       </c>
-      <c r="G800">
-        <v>0</v>
+      <c r="G800" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="801" spans="1:7" x14ac:dyDescent="0.4">
@@ -18870,14 +18870,14 @@
       <c r="C804" s="2">
         <v>5</v>
       </c>
-      <c r="D804" s="1">
-        <v>1</v>
+      <c r="D804">
+        <v>0</v>
       </c>
       <c r="E804" s="1">
         <v>1</v>
       </c>
-      <c r="F804">
-        <v>0</v>
+      <c r="F804" s="1">
+        <v>1</v>
       </c>
       <c r="G804">
         <v>0</v>
@@ -18893,8 +18893,8 @@
       <c r="C805" s="2">
         <v>6</v>
       </c>
-      <c r="D805">
-        <v>0</v>
+      <c r="D805" s="1">
+        <v>1</v>
       </c>
       <c r="E805">
         <v>0</v>
@@ -18919,8 +18919,8 @@
       <c r="D806">
         <v>0</v>
       </c>
-      <c r="E806">
-        <v>0</v>
+      <c r="E806" s="1">
+        <v>1</v>
       </c>
       <c r="F806">
         <v>0</v>
@@ -18945,8 +18945,8 @@
       <c r="E807">
         <v>0</v>
       </c>
-      <c r="F807">
-        <v>0</v>
+      <c r="F807" s="1">
+        <v>1</v>
       </c>
       <c r="G807">
         <v>0</v>
@@ -18962,8 +18962,8 @@
       <c r="C808" s="2">
         <v>1</v>
       </c>
-      <c r="D808" s="1">
-        <v>1</v>
+      <c r="D808">
+        <v>0</v>
       </c>
       <c r="E808">
         <v>0</v>
@@ -18971,8 +18971,8 @@
       <c r="F808">
         <v>0</v>
       </c>
-      <c r="G808">
-        <v>0</v>
+      <c r="G808" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="809" spans="1:7" x14ac:dyDescent="0.4">

</xml_diff>

<commit_message>
permission to dance. Medium 추가
</commit_message>
<xml_diff>
--- a/NoteMaps/PTD_BTS.xlsx
+++ b/NoteMaps/PTD_BTS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eogus\source\repos\RhythmGame\NoteMaps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29A93F82-9052-4D23-9FAD-B184B2EAC20E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D31A9BE-C6AC-4665-AE2F-29BABE5A1ECE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{FBD1AADC-AD03-4139-A607-30D499883534}"/>
   </bookViews>
@@ -482,8 +482,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{597C38B7-F2CF-4951-BED7-7D28309F5979}">
   <dimension ref="A1:G1063"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A841" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H806" sqref="H806"/>
+    <sheetView tabSelected="1" topLeftCell="A739" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I752" sqref="I752"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -18893,8 +18893,8 @@
       <c r="C805" s="2">
         <v>6</v>
       </c>
-      <c r="D805" s="1">
-        <v>1</v>
+      <c r="D805">
+        <v>0</v>
       </c>
       <c r="E805">
         <v>0</v>
@@ -18919,8 +18919,8 @@
       <c r="D806">
         <v>0</v>
       </c>
-      <c r="E806" s="1">
-        <v>1</v>
+      <c r="E806">
+        <v>0</v>
       </c>
       <c r="F806">
         <v>0</v>
@@ -18945,8 +18945,8 @@
       <c r="E807">
         <v>0</v>
       </c>
-      <c r="F807" s="1">
-        <v>1</v>
+      <c r="F807">
+        <v>0</v>
       </c>
       <c r="G807">
         <v>0</v>
@@ -18962,14 +18962,14 @@
       <c r="C808" s="2">
         <v>1</v>
       </c>
-      <c r="D808">
-        <v>0</v>
+      <c r="D808" s="1">
+        <v>1</v>
       </c>
       <c r="E808">
         <v>0</v>
       </c>
-      <c r="F808">
-        <v>0</v>
+      <c r="F808" s="1">
+        <v>1</v>
       </c>
       <c r="G808" s="1">
         <v>1</v>
@@ -19244,11 +19244,11 @@
       <c r="E820">
         <v>0</v>
       </c>
-      <c r="F820">
-        <v>0</v>
-      </c>
-      <c r="G820" s="1">
-        <v>1</v>
+      <c r="F820" s="1">
+        <v>1</v>
+      </c>
+      <c r="G820">
+        <v>0</v>
       </c>
     </row>
     <row r="821" spans="1:7" x14ac:dyDescent="0.4">
@@ -19336,11 +19336,11 @@
       <c r="E824">
         <v>0</v>
       </c>
-      <c r="F824">
-        <v>0</v>
-      </c>
-      <c r="G824" s="1">
-        <v>1</v>
+      <c r="F824" s="1">
+        <v>1</v>
+      </c>
+      <c r="G824">
+        <v>0</v>
       </c>
     </row>
     <row r="825" spans="1:7" x14ac:dyDescent="0.4">
@@ -19382,8 +19382,8 @@
       <c r="E826">
         <v>0</v>
       </c>
-      <c r="F826" s="1">
-        <v>1</v>
+      <c r="F826">
+        <v>0</v>
       </c>
       <c r="G826">
         <v>0</v>
@@ -19425,11 +19425,11 @@
       <c r="D828" s="1">
         <v>1</v>
       </c>
-      <c r="E828" s="1">
-        <v>1</v>
-      </c>
-      <c r="F828">
-        <v>0</v>
+      <c r="E828">
+        <v>0</v>
+      </c>
+      <c r="F828" s="1">
+        <v>1</v>
       </c>
       <c r="G828">
         <v>0</v>
@@ -19474,8 +19474,8 @@
       <c r="E830">
         <v>0</v>
       </c>
-      <c r="F830" s="1">
-        <v>1</v>
+      <c r="F830">
+        <v>0</v>
       </c>
       <c r="G830">
         <v>0</v>
@@ -19615,8 +19615,8 @@
       <c r="F836">
         <v>0</v>
       </c>
-      <c r="G836">
-        <v>0</v>
+      <c r="G836" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="837" spans="1:7" x14ac:dyDescent="0.4">
@@ -19799,8 +19799,8 @@
       <c r="F844">
         <v>0</v>
       </c>
-      <c r="G844" s="1">
-        <v>1</v>
+      <c r="G844">
+        <v>0</v>
       </c>
     </row>
     <row r="845" spans="1:7" x14ac:dyDescent="0.4">
@@ -19891,8 +19891,8 @@
       <c r="F848">
         <v>0</v>
       </c>
-      <c r="G848" s="1">
-        <v>1</v>
+      <c r="G848">
+        <v>0</v>
       </c>
     </row>
     <row r="849" spans="1:7" x14ac:dyDescent="0.4">
@@ -20029,8 +20029,8 @@
       <c r="F854">
         <v>0</v>
       </c>
-      <c r="G854">
-        <v>0</v>
+      <c r="G854" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="855" spans="1:7" x14ac:dyDescent="0.4">
@@ -20072,11 +20072,11 @@
       <c r="E856">
         <v>0</v>
       </c>
-      <c r="F856">
-        <v>0</v>
-      </c>
-      <c r="G856" s="1">
-        <v>1</v>
+      <c r="F856" s="1">
+        <v>1</v>
+      </c>
+      <c r="G856">
+        <v>0</v>
       </c>
     </row>
     <row r="857" spans="1:7" x14ac:dyDescent="0.4">
@@ -20164,8 +20164,8 @@
       <c r="E860">
         <v>0</v>
       </c>
-      <c r="F860" s="1">
-        <v>1</v>
+      <c r="F860">
+        <v>0</v>
       </c>
       <c r="G860">
         <v>0</v>
@@ -20256,8 +20256,8 @@
       <c r="E864" s="1">
         <v>1</v>
       </c>
-      <c r="F864">
-        <v>0</v>
+      <c r="F864" s="1">
+        <v>1</v>
       </c>
       <c r="G864">
         <v>0</v>
@@ -20348,11 +20348,11 @@
       <c r="E868">
         <v>0</v>
       </c>
-      <c r="F868" s="1">
-        <v>1</v>
-      </c>
-      <c r="G868">
-        <v>0</v>
+      <c r="F868">
+        <v>0</v>
+      </c>
+      <c r="G868" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="869" spans="1:7" x14ac:dyDescent="0.4">

</xml_diff>